<commit_message>
Project Original + Entrega 4
</commit_message>
<xml_diff>
--- a/Risk Register.xlsx
+++ b/Risk Register.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Rafael Soares\Documents\GitHub\GPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Catarina\Documents\FACULDADE\MEIC\GPI\ProjetoAtual\GPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89E8353-254A-4FC3-8D2F-A7385FC5AD35}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFA0E6B-7A07-47DF-9E32-28560AC99047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0A3FD882-63F8-436E-92DC-10A7B7DE5E2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{0A3FD882-63F8-436E-92DC-10A7B7DE5E2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
   <si>
     <t>Risk</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Treatment</t>
-  </si>
-  <si>
-    <t>ID</t>
   </si>
   <si>
     <t>VL</t>
@@ -237,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -252,6 +249,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -274,7 +274,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -575,32 +575,31 @@
   </sheetPr>
   <dimension ref="B2:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="61" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.734375" customWidth="1"/>
-    <col min="3" max="3" width="12.7890625" customWidth="1"/>
-    <col min="4" max="4" width="13.5234375" customWidth="1"/>
-    <col min="5" max="5" width="3.1015625" customWidth="1"/>
-    <col min="6" max="6" width="3.05078125" customWidth="1"/>
-    <col min="7" max="7" width="3" customWidth="1"/>
-    <col min="8" max="8" width="2.89453125" customWidth="1"/>
-    <col min="9" max="9" width="3.05078125" customWidth="1"/>
-    <col min="10" max="10" width="3.734375" customWidth="1"/>
-    <col min="11" max="11" width="2.15625" customWidth="1"/>
-    <col min="12" max="12" width="2.578125" customWidth="1"/>
-    <col min="13" max="13" width="2.41796875" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="3.140625" customWidth="1"/>
+    <col min="6" max="7" width="3" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+    <col min="9" max="9" width="3" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" customWidth="1"/>
+    <col min="11" max="11" width="2.140625" customWidth="1"/>
+    <col min="12" max="12" width="2.5703125" customWidth="1"/>
+    <col min="13" max="13" width="2.42578125" customWidth="1"/>
     <col min="14" max="14" width="3" customWidth="1"/>
-    <col min="15" max="15" width="32.7890625" customWidth="1"/>
-    <col min="16" max="16" width="11.15625" customWidth="1"/>
-    <col min="17" max="17" width="19.26171875" customWidth="1"/>
-    <col min="18" max="18" width="11.578125" customWidth="1"/>
+    <col min="15" max="15" width="32.85546875" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -610,130 +609,130 @@
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
       <c r="O2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="7"/>
+      <c r="Q2" s="8"/>
       <c r="R2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="3" t="s">
-        <v>7</v>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="3" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="4" spans="2:18" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="3">
-        <v>1</v>
+    <row r="4" spans="2:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="Q4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="R4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="3">
-        <v>2</v>
+    <row r="5" spans="2:18" ht="120" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -742,36 +741,36 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N5" s="5"/>
       <c r="O5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="R5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:18" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="3">
-        <v>3</v>
+    <row r="6" spans="2:18" ht="150" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -779,73 +778,73 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N6" s="5"/>
       <c r="O6" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="3">
-        <v>4</v>
+    <row r="7" spans="2:18" ht="120" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="3">
-        <v>5</v>
+    <row r="8" spans="2:18" ht="150" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -854,59 +853,59 @@
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Q8" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="R8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:18" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:18" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update risk register to reflect updates on project status
</commit_message>
<xml_diff>
--- a/Risk Register.xlsx
+++ b/Risk Register.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Catarina\Documents\FACULDADE\MEIC\GPI\ProjetoAtual\GPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\GPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFA0E6B-7A07-47DF-9E32-28560AC99047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C125B3A7-3B77-4961-97B0-DB9966068D69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{0A3FD882-63F8-436E-92DC-10A7B7DE5E2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A3FD882-63F8-436E-92DC-10A7B7DE5E2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -175,8 +175,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -234,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -255,6 +263,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -575,8 +586,8 @@
   </sheetPr>
   <dimension ref="B2:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="61" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:R9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,10 +741,10 @@
       <c r="D5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="E5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -767,11 +778,11 @@
       <c r="D6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -842,19 +853,17 @@
         <v>40</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5" t="s">
+      <c r="F8" s="9" t="s">
         <v>18</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+      <c r="L8" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="M8" s="5"/>
-      <c r="N8" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="O8" s="4" t="s">
         <v>24</v>
       </c>

</xml_diff>